<commit_message>
1. Initialised esm2.1 from CMIP5 documents.  2. Updated spreadsheets to latest version.
</commit_message>
<xml_diff>
--- a/cmip6/models/cnrm-cm6-1/cmip6_cnrm-cerfacs_cnrm-cm6-1_atmos.xlsx
+++ b/cmip6/models/cnrm-cm6-1/cmip6_cnrm-cerfacs_cnrm-cm6-1_atmos.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1848" uniqueCount="1140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1835" uniqueCount="1136">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -2361,9 +2361,6 @@
     <t>cmip6.atmos.microphysics_precipitation.large_scale_cloud_microphysics.processes</t>
   </si>
   <si>
-    <t>Cloud droplets</t>
-  </si>
-  <si>
     <t>mixed phase</t>
   </si>
   <si>
@@ -2388,9 +2385,6 @@
     <t>effect of graupel</t>
   </si>
   <si>
-    <t>Cloud ice</t>
-  </si>
-  <si>
     <t>7.1.1</t>
   </si>
   <si>
@@ -2928,9 +2922,6 @@
     <t>cmip6.atmos.observation_simulation.lidar_inputs.overlap</t>
   </si>
   <si>
-    <t>Max</t>
-  </si>
-  <si>
     <t>max</t>
   </si>
   <si>
@@ -3436,9 +3427,6 @@
   </si>
   <si>
     <t>cmip6.atmos.natural_forcing.volcanoes_treatment.volcanoes_implementation</t>
-  </si>
-  <si>
-    <t>Stratospheric aerosols optical thickness</t>
   </si>
   <si>
     <t>high frequency solar constant anomaly</t>
@@ -4105,20 +4093,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>45</v>
@@ -4129,10 +4117,10 @@
         <v>46</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
@@ -4140,7 +4128,7 @@
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>56</v>
@@ -4151,10 +4139,10 @@
         <v>46</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
@@ -4167,23 +4155,23 @@
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="13" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="24" customHeight="1">
@@ -4191,10 +4179,10 @@
         <v>62</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="24" customHeight="1">
@@ -4204,16 +4192,16 @@
     </row>
     <row r="20" spans="1:30" ht="24" customHeight="1">
       <c r="B20" s="11" t="s">
+        <v>897</v>
+      </c>
+      <c r="AA20" s="6" t="s">
+        <v>898</v>
+      </c>
+      <c r="AB20" s="6" t="s">
+        <v>897</v>
+      </c>
+      <c r="AC20" s="6" t="s">
         <v>899</v>
-      </c>
-      <c r="AA20" s="6" t="s">
-        <v>900</v>
-      </c>
-      <c r="AB20" s="6" t="s">
-        <v>899</v>
-      </c>
-      <c r="AC20" s="6" t="s">
-        <v>901</v>
       </c>
       <c r="AD20" s="6" t="s">
         <v>67</v>
@@ -4221,16 +4209,16 @@
     </row>
     <row r="21" spans="1:30" ht="24" customHeight="1">
       <c r="B21" s="11" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="AA21" s="6" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="AB21" s="6" t="s">
+        <v>897</v>
+      </c>
+      <c r="AC21" s="6" t="s">
         <v>899</v>
-      </c>
-      <c r="AC21" s="6" t="s">
-        <v>901</v>
       </c>
       <c r="AD21" s="6" t="s">
         <v>67</v>
@@ -4238,10 +4226,10 @@
     </row>
     <row r="23" spans="1:30" ht="24" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="24" spans="1:30" ht="24" customHeight="1">
@@ -4249,21 +4237,21 @@
         <v>62</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="25" spans="1:30" ht="24" customHeight="1">
       <c r="B25" s="11" t="s">
+        <v>905</v>
+      </c>
+      <c r="AA25" s="6" t="s">
+        <v>906</v>
+      </c>
+      <c r="AB25" s="6" t="s">
         <v>907</v>
-      </c>
-      <c r="AA25" s="6" t="s">
-        <v>908</v>
-      </c>
-      <c r="AB25" s="6" t="s">
-        <v>909</v>
       </c>
       <c r="AC25" s="6" t="s">
         <v>67</v>
@@ -4271,23 +4259,23 @@
     </row>
     <row r="28" spans="1:30" ht="24" customHeight="1">
       <c r="A28" s="12" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="24" customHeight="1">
       <c r="B29" s="13" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
     </row>
     <row r="31" spans="1:30" ht="24" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
     </row>
     <row r="32" spans="1:30" ht="24" customHeight="1">
@@ -4295,21 +4283,21 @@
         <v>62</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
     </row>
     <row r="33" spans="1:29" ht="24" customHeight="1">
       <c r="B33" s="11" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="AA33" s="6" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="AB33" s="6" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="AC33" s="6" t="s">
         <v>67</v>
@@ -4317,10 +4305,10 @@
     </row>
     <row r="35" spans="1:29" ht="24" customHeight="1">
       <c r="A35" s="9" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="24" customHeight="1">
@@ -4328,10 +4316,10 @@
         <v>96</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="24" customHeight="1">
@@ -4339,10 +4327,10 @@
     </row>
     <row r="39" spans="1:29" ht="24" customHeight="1">
       <c r="A39" s="9" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="24" customHeight="1">
@@ -4350,10 +4338,10 @@
         <v>96</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="24" customHeight="1">
@@ -4363,10 +4351,10 @@
     </row>
     <row r="43" spans="1:29" ht="24" customHeight="1">
       <c r="A43" s="9" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="24" customHeight="1">
@@ -4374,10 +4362,10 @@
         <v>96</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="24" customHeight="1">
@@ -4387,34 +4375,34 @@
     </row>
     <row r="48" spans="1:29" ht="24" customHeight="1">
       <c r="A48" s="12" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="49" spans="1:29" ht="24" customHeight="1">
       <c r="B49" s="13" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="51" spans="1:29" ht="24" customHeight="1">
       <c r="A51" s="9" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="52" spans="1:29" ht="24" customHeight="1">
       <c r="A52" s="14" t="s">
+        <v>934</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>935</v>
+      </c>
+      <c r="C52" s="10" t="s">
         <v>936</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>937</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="53" spans="1:29" ht="24" customHeight="1">
@@ -4422,7 +4410,7 @@
     </row>
     <row r="55" spans="1:29" ht="24" customHeight="1">
       <c r="A55" s="9" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>123</v>
@@ -4433,21 +4421,21 @@
         <v>62</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="57" spans="1:29" ht="24" customHeight="1">
       <c r="B57" s="11" t="s">
+        <v>940</v>
+      </c>
+      <c r="AA57" s="6" t="s">
+        <v>941</v>
+      </c>
+      <c r="AB57" s="6" t="s">
         <v>942</v>
-      </c>
-      <c r="AA57" s="6" t="s">
-        <v>943</v>
-      </c>
-      <c r="AB57" s="6" t="s">
-        <v>944</v>
       </c>
       <c r="AC57" s="6" t="s">
         <v>67</v>
@@ -4455,10 +4443,10 @@
     </row>
     <row r="59" spans="1:29" ht="24" customHeight="1">
       <c r="A59" s="9" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
     </row>
     <row r="60" spans="1:29" ht="24" customHeight="1">
@@ -4466,10 +4454,10 @@
         <v>101</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="61" spans="1:29" ht="24" customHeight="1">
@@ -4479,10 +4467,10 @@
     </row>
     <row r="63" spans="1:29" ht="24" customHeight="1">
       <c r="A63" s="9" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="64" spans="1:29" ht="24" customHeight="1">
@@ -4490,10 +4478,10 @@
         <v>101</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
     </row>
     <row r="65" spans="1:29" ht="24" customHeight="1">
@@ -4503,23 +4491,23 @@
     </row>
     <row r="68" spans="1:29" ht="24" customHeight="1">
       <c r="A68" s="12" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
     <row r="69" spans="1:29" ht="24" customHeight="1">
       <c r="B69" s="13" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="71" spans="1:29" ht="24" customHeight="1">
       <c r="A71" s="9" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="72" spans="1:29" ht="24" customHeight="1">
@@ -4527,21 +4515,21 @@
         <v>62</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
     </row>
     <row r="73" spans="1:29" ht="24" customHeight="1">
       <c r="B73" s="11" t="s">
+        <v>958</v>
+      </c>
+      <c r="AA73" s="6" t="s">
+        <v>959</v>
+      </c>
+      <c r="AB73" s="6" t="s">
         <v>960</v>
-      </c>
-      <c r="AA73" s="6" t="s">
-        <v>961</v>
-      </c>
-      <c r="AB73" s="6" t="s">
-        <v>962</v>
       </c>
       <c r="AC73" s="6" t="s">
         <v>67</v>
@@ -4549,10 +4537,10 @@
     </row>
     <row r="75" spans="1:29" ht="24" customHeight="1">
       <c r="A75" s="9" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="76" spans="1:29" ht="24" customHeight="1">
@@ -4560,10 +4548,10 @@
         <v>62</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="77" spans="1:29" ht="24" customHeight="1">
@@ -4572,14 +4560,12 @@
       </c>
     </row>
     <row r="78" spans="1:29" ht="24" customHeight="1">
-      <c r="B78" s="11" t="s">
-        <v>967</v>
-      </c>
+      <c r="B78" s="11"/>
       <c r="AA78" s="6" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="AB78" s="6" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="AC78" s="6" t="s">
         <v>67</v>
@@ -4648,20 +4634,20 @@
   <sheetData>
     <row r="1" spans="1:29" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>45</v>
@@ -4672,10 +4658,10 @@
         <v>46</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="24" customHeight="1">
@@ -4683,7 +4669,7 @@
     </row>
     <row r="8" spans="1:29" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>56</v>
@@ -4694,10 +4680,10 @@
         <v>46</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="24" customHeight="1">
@@ -4710,10 +4696,10 @@
     </row>
     <row r="13" spans="1:29" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="24" customHeight="1">
@@ -4721,19 +4707,19 @@
         <v>62</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="24" customHeight="1">
       <c r="B15" s="11"/>
       <c r="AA15" s="6" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="AB15" s="6" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="AC15" s="6" t="s">
         <v>67</v>
@@ -4741,10 +4727,10 @@
     </row>
     <row r="17" spans="1:30" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="24" customHeight="1">
@@ -4752,19 +4738,19 @@
         <v>62</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="24" customHeight="1">
       <c r="B19" s="11"/>
       <c r="AA19" s="6" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="AB19" s="6" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="AC19" s="6" t="s">
         <v>67</v>
@@ -4772,10 +4758,10 @@
     </row>
     <row r="21" spans="1:30" ht="24" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="24" customHeight="1">
@@ -4783,10 +4769,10 @@
         <v>62</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
     </row>
     <row r="23" spans="1:30" ht="24" customHeight="1">
@@ -4796,16 +4782,16 @@
     </row>
     <row r="24" spans="1:30" ht="24" customHeight="1">
       <c r="B24" s="11" t="s">
+        <v>991</v>
+      </c>
+      <c r="AA24" s="6" t="s">
+        <v>992</v>
+      </c>
+      <c r="AB24" s="6" t="s">
+        <v>993</v>
+      </c>
+      <c r="AC24" s="6" t="s">
         <v>994</v>
-      </c>
-      <c r="AA24" s="6" t="s">
-        <v>995</v>
-      </c>
-      <c r="AB24" s="6" t="s">
-        <v>996</v>
-      </c>
-      <c r="AC24" s="6" t="s">
-        <v>997</v>
       </c>
       <c r="AD24" s="6" t="s">
         <v>67</v>
@@ -4813,16 +4799,16 @@
     </row>
     <row r="25" spans="1:30" ht="24" customHeight="1">
       <c r="B25" s="11" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="AA25" s="6" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="AB25" s="6" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="AC25" s="6" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="AD25" s="6" t="s">
         <v>67</v>
@@ -4830,20 +4816,20 @@
     </row>
     <row r="28" spans="1:30" ht="24" customHeight="1">
       <c r="A28" s="12" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="24" customHeight="1">
       <c r="B29" s="13" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
     </row>
     <row r="31" spans="1:30" ht="24" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>45</v>
@@ -4854,10 +4840,10 @@
         <v>46</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="33" spans="1:32" ht="24" customHeight="1">
@@ -4865,10 +4851,10 @@
     </row>
     <row r="35" spans="1:32" ht="24" customHeight="1">
       <c r="A35" s="9" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="36" spans="1:32" ht="24" customHeight="1">
@@ -4876,10 +4862,10 @@
         <v>62</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="37" spans="1:32" ht="24" customHeight="1">
@@ -4889,22 +4875,22 @@
     </row>
     <row r="38" spans="1:32" ht="24" customHeight="1">
       <c r="B38" s="11" t="s">
+        <v>1006</v>
+      </c>
+      <c r="AA38" s="6" t="s">
+        <v>1007</v>
+      </c>
+      <c r="AB38" s="6" t="s">
+        <v>1008</v>
+      </c>
+      <c r="AC38" s="6" t="s">
         <v>1009</v>
       </c>
-      <c r="AA38" s="6" t="s">
+      <c r="AD38" s="6" t="s">
         <v>1010</v>
       </c>
-      <c r="AB38" s="6" t="s">
+      <c r="AE38" s="6" t="s">
         <v>1011</v>
-      </c>
-      <c r="AC38" s="6" t="s">
-        <v>1012</v>
-      </c>
-      <c r="AD38" s="6" t="s">
-        <v>1013</v>
-      </c>
-      <c r="AE38" s="6" t="s">
-        <v>1014</v>
       </c>
       <c r="AF38" s="6" t="s">
         <v>67</v>
@@ -4912,22 +4898,22 @@
     </row>
     <row r="39" spans="1:32" ht="24" customHeight="1">
       <c r="B39" s="11" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
       <c r="AA39" s="6" t="s">
+        <v>1007</v>
+      </c>
+      <c r="AB39" s="6" t="s">
+        <v>1008</v>
+      </c>
+      <c r="AC39" s="6" t="s">
+        <v>1009</v>
+      </c>
+      <c r="AD39" s="6" t="s">
         <v>1010</v>
       </c>
-      <c r="AB39" s="6" t="s">
+      <c r="AE39" s="6" t="s">
         <v>1011</v>
-      </c>
-      <c r="AC39" s="6" t="s">
-        <v>1012</v>
-      </c>
-      <c r="AD39" s="6" t="s">
-        <v>1013</v>
-      </c>
-      <c r="AE39" s="6" t="s">
-        <v>1014</v>
       </c>
       <c r="AF39" s="6" t="s">
         <v>67</v>
@@ -4935,10 +4921,10 @@
     </row>
     <row r="41" spans="1:32" ht="24" customHeight="1">
       <c r="A41" s="9" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="42" spans="1:32" ht="24" customHeight="1">
@@ -4946,10 +4932,10 @@
         <v>62</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="43" spans="1:32" ht="24" customHeight="1">
@@ -4959,13 +4945,13 @@
     </row>
     <row r="44" spans="1:32" ht="24" customHeight="1">
       <c r="B44" s="11" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="AA44" s="6" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="AB44" s="6" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="AC44" s="6" t="s">
         <v>67</v>
@@ -4973,10 +4959,10 @@
     </row>
     <row r="46" spans="1:32" ht="24" customHeight="1">
       <c r="A46" s="9" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="47" spans="1:32" ht="24" customHeight="1">
@@ -4984,24 +4970,24 @@
         <v>62</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="48" spans="1:32" ht="24" customHeight="1">
       <c r="B48" s="11" t="s">
+        <v>1024</v>
+      </c>
+      <c r="AA48" s="6" t="s">
+        <v>1025</v>
+      </c>
+      <c r="AB48" s="6" t="s">
+        <v>1026</v>
+      </c>
+      <c r="AC48" s="6" t="s">
         <v>1027</v>
-      </c>
-      <c r="AA48" s="6" t="s">
-        <v>1028</v>
-      </c>
-      <c r="AB48" s="6" t="s">
-        <v>1029</v>
-      </c>
-      <c r="AC48" s="6" t="s">
-        <v>1030</v>
       </c>
       <c r="AD48" s="6" t="s">
         <v>67</v>
@@ -5009,10 +4995,10 @@
     </row>
     <row r="50" spans="1:32" ht="24" customHeight="1">
       <c r="A50" s="9" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="51" spans="1:32" ht="24" customHeight="1">
@@ -5020,19 +5006,19 @@
         <v>62</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="52" spans="1:32" ht="24" customHeight="1">
       <c r="B52" s="11"/>
       <c r="AA52" s="6" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="AB52" s="6" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="AC52" s="6" t="s">
         <v>177</v>
@@ -5041,7 +5027,7 @@
         <v>327</v>
       </c>
       <c r="AE52" s="6" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="AF52" s="6" t="s">
         <v>67</v>
@@ -5049,20 +5035,20 @@
     </row>
     <row r="55" spans="1:32" ht="24" customHeight="1">
       <c r="A55" s="12" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="56" spans="1:32" ht="24" customHeight="1">
       <c r="B56" s="13" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="58" spans="1:32" ht="24" customHeight="1">
       <c r="A58" s="9" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>45</v>
@@ -5073,10 +5059,10 @@
         <v>46</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="60" spans="1:32" ht="24" customHeight="1">
@@ -5084,10 +5070,10 @@
     </row>
     <row r="62" spans="1:32" ht="24" customHeight="1">
       <c r="A62" s="9" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="63" spans="1:32" ht="24" customHeight="1">
@@ -5095,10 +5081,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="64" spans="1:32" ht="24" customHeight="1">
@@ -5109,13 +5095,13 @@
     <row r="65" spans="1:32" ht="24" customHeight="1">
       <c r="B65" s="11"/>
       <c r="AA65" s="6" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="AB65" s="6" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="AC65" s="6" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="AD65" s="6" t="s">
         <v>67</v>
@@ -5123,10 +5109,10 @@
     </row>
     <row r="67" spans="1:32" ht="24" customHeight="1">
       <c r="A67" s="9" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="68" spans="1:32" ht="24" customHeight="1">
@@ -5134,10 +5120,10 @@
         <v>62</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="69" spans="1:32" ht="24" customHeight="1">
@@ -5148,18 +5134,18 @@
     <row r="70" spans="1:32" ht="24" customHeight="1">
       <c r="B70" s="11"/>
       <c r="AA70" s="6" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="AB70" s="6" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="72" spans="1:32" ht="24" customHeight="1">
       <c r="A72" s="9" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="73" spans="1:32" ht="24" customHeight="1">
@@ -5167,19 +5153,19 @@
         <v>62</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="74" spans="1:32" ht="24" customHeight="1">
       <c r="B74" s="11"/>
       <c r="AA74" s="6" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="AB74" s="6" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="AC74" s="6" t="s">
         <v>67</v>
@@ -5187,10 +5173,10 @@
     </row>
     <row r="76" spans="1:32" ht="24" customHeight="1">
       <c r="A76" s="9" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="77" spans="1:32" ht="24" customHeight="1">
@@ -5198,19 +5184,19 @@
         <v>62</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="78" spans="1:32" ht="24" customHeight="1">
       <c r="B78" s="11"/>
       <c r="AA78" s="6" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="AB78" s="6" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="AC78" s="6" t="s">
         <v>177</v>
@@ -5219,7 +5205,7 @@
         <v>327</v>
       </c>
       <c r="AE78" s="6" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="AF78" s="6" t="s">
         <v>67</v>
@@ -5287,20 +5273,20 @@
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>45</v>
@@ -5311,10 +5297,10 @@
         <v>46</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
@@ -5322,7 +5308,7 @@
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>56</v>
@@ -5333,10 +5319,10 @@
         <v>46</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" customHeight="1">
@@ -5349,23 +5335,23 @@
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1">
       <c r="B15" s="13" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="24" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="24" customHeight="1">
@@ -5373,10 +5359,10 @@
         <v>62</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="24" customHeight="1">
@@ -5387,13 +5373,13 @@
     <row r="20" spans="1:30" ht="24" customHeight="1">
       <c r="B20" s="11"/>
       <c r="AA20" s="6" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="AB20" s="6" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="AC20" s="6" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="AD20" s="6" t="s">
         <v>67</v>
@@ -5401,20 +5387,20 @@
     </row>
     <row r="23" spans="1:30" ht="24" customHeight="1">
       <c r="A23" s="12" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="24" spans="1:30" ht="24" customHeight="1">
       <c r="B24" s="13" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="24" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>123</v>
@@ -5425,40 +5411,40 @@
         <v>62</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="28" spans="1:30" ht="24" customHeight="1">
       <c r="B28" s="11" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="AA28" s="6" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="AB28" s="6" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="30" spans="1:30" ht="24" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="31" spans="1:30" ht="24" customHeight="1">
       <c r="A31" s="14" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="32" spans="1:30" ht="24" customHeight="1">
@@ -5466,10 +5452,10 @@
     </row>
     <row r="34" spans="1:28" ht="24" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="35" spans="1:28" ht="24" customHeight="1">
@@ -5477,33 +5463,33 @@
         <v>46</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="36" spans="1:28" ht="24" customHeight="1">
       <c r="B36" s="11" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="39" spans="1:28" ht="24" customHeight="1">
       <c r="A39" s="12" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="40" spans="1:28" ht="24" customHeight="1">
       <c r="B40" s="13" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="42" spans="1:28" ht="24" customHeight="1">
       <c r="A42" s="9" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>123</v>
@@ -5514,29 +5500,29 @@
         <v>62</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="44" spans="1:28" ht="24" customHeight="1">
       <c r="B44" s="11" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="AA44" s="6" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="AB44" s="6" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="46" spans="1:28" ht="24" customHeight="1">
       <c r="A46" s="9" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="47" spans="1:28" ht="24" customHeight="1">
@@ -5544,10 +5530,10 @@
         <v>96</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="48" spans="1:28" ht="24" customHeight="1">
@@ -5555,10 +5541,10 @@
     </row>
     <row r="50" spans="1:29" ht="24" customHeight="1">
       <c r="A50" s="9" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="51" spans="1:29" ht="24" customHeight="1">
@@ -5566,23 +5552,23 @@
         <v>46</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="52" spans="1:29" ht="24" customHeight="1">
       <c r="B52" s="11" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="54" spans="1:29" ht="24" customHeight="1">
       <c r="A54" s="9" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="55" spans="1:29" ht="24" customHeight="1">
@@ -5590,19 +5576,19 @@
         <v>62</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="56" spans="1:29" ht="24" customHeight="1">
       <c r="B56" s="11"/>
       <c r="AA56" s="6" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="AB56" s="6" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="AC56" s="6" t="s">
         <v>67</v>
@@ -5610,23 +5596,23 @@
     </row>
     <row r="59" spans="1:29" ht="24" customHeight="1">
       <c r="A59" s="12" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="60" spans="1:29" ht="24" customHeight="1">
       <c r="B60" s="13" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="62" spans="1:29" ht="24" customHeight="1">
       <c r="A62" s="9" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="63" spans="1:29" ht="24" customHeight="1">
@@ -5634,10 +5620,10 @@
         <v>101</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="64" spans="1:29" ht="24" customHeight="1">
@@ -5647,23 +5633,23 @@
     </row>
     <row r="67" spans="1:29" ht="24" customHeight="1">
       <c r="A67" s="12" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="68" spans="1:29" ht="24" customHeight="1">
       <c r="B68" s="13" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="70" spans="1:29" ht="24" customHeight="1">
       <c r="A70" s="9" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="71" spans="1:29" ht="24" customHeight="1">
@@ -5671,10 +5657,10 @@
         <v>46</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="72" spans="1:29" ht="24" customHeight="1">
@@ -5687,10 +5673,10 @@
     </row>
     <row r="75" spans="1:29" ht="24" customHeight="1">
       <c r="A75" s="9" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="76" spans="1:29" ht="24" customHeight="1">
@@ -5698,21 +5684,19 @@
         <v>62</v>
       </c>
       <c r="B76" s="10" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="77" spans="1:29" ht="24" customHeight="1">
+      <c r="B77" s="11"/>
+      <c r="AA77" s="6" t="s">
+        <v>1134</v>
+      </c>
+      <c r="AB77" s="6" t="s">
         <v>1135</v>
-      </c>
-      <c r="C76" s="10" t="s">
-        <v>1136</v>
-      </c>
-    </row>
-    <row r="77" spans="1:29" ht="24" customHeight="1">
-      <c r="B77" s="11" t="s">
-        <v>1137</v>
-      </c>
-      <c r="AA77" s="6" t="s">
-        <v>1138</v>
-      </c>
-      <c r="AB77" s="6" t="s">
-        <v>1139</v>
       </c>
       <c r="AC77" s="6" t="s">
         <v>67</v>
@@ -10744,7 +10728,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD39"/>
+  <dimension ref="A1:XFD38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10981,71 +10965,37 @@
       </c>
     </row>
     <row r="38" spans="1:35" ht="24" customHeight="1">
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="11"/>
+      <c r="AA38" s="6" t="s">
         <v>778</v>
       </c>
-      <c r="AA38" s="6" t="s">
+      <c r="AB38" s="6" t="s">
         <v>779</v>
       </c>
-      <c r="AB38" s="6" t="s">
+      <c r="AC38" s="6" t="s">
         <v>780</v>
       </c>
-      <c r="AC38" s="6" t="s">
+      <c r="AD38" s="6" t="s">
         <v>781</v>
       </c>
-      <c r="AD38" s="6" t="s">
+      <c r="AE38" s="6" t="s">
         <v>782</v>
       </c>
-      <c r="AE38" s="6" t="s">
+      <c r="AF38" s="6" t="s">
         <v>783</v>
       </c>
-      <c r="AF38" s="6" t="s">
+      <c r="AG38" s="6" t="s">
         <v>784</v>
       </c>
-      <c r="AG38" s="6" t="s">
+      <c r="AH38" s="6" t="s">
         <v>785</v>
-      </c>
-      <c r="AH38" s="6" t="s">
-        <v>786</v>
       </c>
       <c r="AI38" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:35" ht="24" customHeight="1">
-      <c r="B39" s="11" t="s">
-        <v>787</v>
-      </c>
-      <c r="AA39" s="6" t="s">
-        <v>779</v>
-      </c>
-      <c r="AB39" s="6" t="s">
-        <v>780</v>
-      </c>
-      <c r="AC39" s="6" t="s">
-        <v>781</v>
-      </c>
-      <c r="AD39" s="6" t="s">
-        <v>782</v>
-      </c>
-      <c r="AE39" s="6" t="s">
-        <v>783</v>
-      </c>
-      <c r="AF39" s="6" t="s">
-        <v>784</v>
-      </c>
-      <c r="AG39" s="6" t="s">
-        <v>785</v>
-      </c>
-      <c r="AH39" s="6" t="s">
-        <v>786</v>
-      </c>
-      <c r="AI39" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
       <formula1>AA24:AE24</formula1>
     </dataValidation>
@@ -11054,9 +11004,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38">
       <formula1>AA38:AI38</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39">
-      <formula1>AA39:AI39</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11079,20 +11026,20 @@
   <sheetData>
     <row r="1" spans="1:29" ht="24" customHeight="1">
       <c r="A1" s="12" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="24" customHeight="1">
       <c r="B2" s="13" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="24" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>45</v>
@@ -11103,10 +11050,10 @@
         <v>46</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="24" customHeight="1">
@@ -11114,7 +11061,7 @@
     </row>
     <row r="8" spans="1:29" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>56</v>
@@ -11125,10 +11072,10 @@
         <v>46</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="24" customHeight="1">
@@ -11141,7 +11088,7 @@
     </row>
     <row r="13" spans="1:29" ht="24" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>173</v>
@@ -11152,10 +11099,10 @@
         <v>62</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="24" customHeight="1">
@@ -11166,10 +11113,10 @@
     <row r="16" spans="1:29" ht="24" customHeight="1">
       <c r="B16" s="11"/>
       <c r="AA16" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="AB16" s="6" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="AC16" s="6" t="s">
         <v>67</v>
@@ -11177,10 +11124,10 @@
     </row>
     <row r="18" spans="1:34" ht="24" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="24" customHeight="1">
@@ -11188,20 +11135,20 @@
         <v>46</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="20" spans="1:34" ht="24" customHeight="1">
       <c r="B20" s="11" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="22" spans="1:34" ht="24" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>697</v>
@@ -11212,10 +11159,10 @@
         <v>62</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="24" spans="1:34" ht="24" customHeight="1">
@@ -11225,7 +11172,7 @@
     </row>
     <row r="25" spans="1:34" ht="24" customHeight="1">
       <c r="B25" s="11" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="AA25" s="6" t="s">
         <v>703</v>
@@ -11234,7 +11181,7 @@
         <v>704</v>
       </c>
       <c r="AC25" s="6" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="AD25" s="6" t="s">
         <v>67</v>
@@ -11242,7 +11189,7 @@
     </row>
     <row r="27" spans="1:34" ht="24" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>245</v>
@@ -11253,10 +11200,10 @@
         <v>62</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="29" spans="1:34" ht="24" customHeight="1">
@@ -11267,25 +11214,25 @@
     <row r="30" spans="1:34" ht="24" customHeight="1">
       <c r="B30" s="11"/>
       <c r="AA30" s="6" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="AB30" s="6" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="AC30" s="6" t="s">
         <v>398</v>
       </c>
       <c r="AD30" s="6" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="AE30" s="6" t="s">
         <v>764</v>
       </c>
       <c r="AF30" s="6" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="AG30" s="6" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="AH30" s="6" t="s">
         <v>67</v>
@@ -11293,10 +11240,10 @@
     </row>
     <row r="32" spans="1:34" ht="24" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
     </row>
     <row r="33" spans="1:32" ht="24" customHeight="1">
@@ -11304,10 +11251,10 @@
         <v>62</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="24" customHeight="1">
@@ -11318,43 +11265,43 @@
     <row r="35" spans="1:32" ht="24" customHeight="1">
       <c r="B35" s="11"/>
       <c r="AA35" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="AB35" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="AC35" s="6" t="s">
         <v>824</v>
       </c>
-      <c r="AB35" s="6" t="s">
+      <c r="AD35" s="6" t="s">
         <v>825</v>
       </c>
-      <c r="AC35" s="6" t="s">
+      <c r="AE35" s="6" t="s">
         <v>826</v>
       </c>
-      <c r="AD35" s="6" t="s">
+      <c r="AF35" s="6" t="s">
         <v>827</v>
-      </c>
-      <c r="AE35" s="6" t="s">
-        <v>828</v>
-      </c>
-      <c r="AF35" s="6" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="38" spans="1:32" ht="24" customHeight="1">
       <c r="A38" s="12" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="39" spans="1:32" ht="24" customHeight="1">
       <c r="B39" s="13" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
     </row>
     <row r="41" spans="1:32" ht="24" customHeight="1">
       <c r="A41" s="9" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
     </row>
     <row r="42" spans="1:32" ht="24" customHeight="1">
@@ -11362,25 +11309,25 @@
         <v>62</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="43" spans="1:32" ht="24" customHeight="1">
       <c r="B43" s="11"/>
       <c r="AA43" s="6" t="s">
+        <v>835</v>
+      </c>
+      <c r="AB43" s="6" t="s">
+        <v>836</v>
+      </c>
+      <c r="AC43" s="6" t="s">
         <v>837</v>
       </c>
-      <c r="AB43" s="6" t="s">
+      <c r="AD43" s="6" t="s">
         <v>838</v>
-      </c>
-      <c r="AC43" s="6" t="s">
-        <v>839</v>
-      </c>
-      <c r="AD43" s="6" t="s">
-        <v>840</v>
       </c>
       <c r="AE43" s="6" t="s">
         <v>67</v>
@@ -11388,7 +11335,7 @@
     </row>
     <row r="45" spans="1:32" ht="24" customHeight="1">
       <c r="A45" s="9" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>550</v>
@@ -11399,10 +11346,10 @@
         <v>46</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="47" spans="1:32" ht="24" customHeight="1">
@@ -11410,20 +11357,20 @@
     </row>
     <row r="50" spans="1:28" ht="24" customHeight="1">
       <c r="A50" s="12" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
     </row>
     <row r="51" spans="1:28" ht="24" customHeight="1">
       <c r="B51" s="13" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
     </row>
     <row r="53" spans="1:28" ht="24" customHeight="1">
       <c r="A53" s="9" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>123</v>
@@ -11434,29 +11381,29 @@
         <v>62</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="55" spans="1:28" ht="24" customHeight="1">
       <c r="B55" s="11" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="AA55" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="AB55" s="6" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="57" spans="1:28" ht="24" customHeight="1">
       <c r="A57" s="9" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="58" spans="1:28" ht="24" customHeight="1">
@@ -11464,23 +11411,23 @@
         <v>46</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="59" spans="1:28" ht="24" customHeight="1">
       <c r="B59" s="11" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="61" spans="1:28" ht="24" customHeight="1">
       <c r="A61" s="9" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="62" spans="1:28" ht="24" customHeight="1">
@@ -11488,10 +11435,10 @@
         <v>96</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="63" spans="1:28" ht="24" customHeight="1">
@@ -11501,10 +11448,10 @@
     </row>
     <row r="65" spans="1:29" ht="24" customHeight="1">
       <c r="A65" s="9" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="66" spans="1:29" ht="24" customHeight="1">
@@ -11512,10 +11459,10 @@
         <v>62</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="67" spans="1:29" ht="24" customHeight="1">
@@ -11525,34 +11472,34 @@
     </row>
     <row r="68" spans="1:29" ht="24" customHeight="1">
       <c r="B68" s="11" t="s">
+        <v>862</v>
+      </c>
+      <c r="AA68" s="6" t="s">
+        <v>863</v>
+      </c>
+      <c r="AB68" s="6" t="s">
         <v>864</v>
       </c>
-      <c r="AA68" s="6" t="s">
+      <c r="AC68" s="6" t="s">
         <v>865</v>
-      </c>
-      <c r="AB68" s="6" t="s">
-        <v>866</v>
-      </c>
-      <c r="AC68" s="6" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="71" spans="1:29" ht="24" customHeight="1">
       <c r="A71" s="12" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="72" spans="1:29" ht="24" customHeight="1">
       <c r="B72" s="13" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="74" spans="1:29" ht="24" customHeight="1">
       <c r="A74" s="9" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="B74" s="9" t="s">
         <v>123</v>
@@ -11563,27 +11510,27 @@
         <v>62</v>
       </c>
       <c r="B75" s="10" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="76" spans="1:29" ht="24" customHeight="1">
       <c r="B76" s="11"/>
       <c r="AA76" s="6" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="AB76" s="6" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="78" spans="1:29" ht="24" customHeight="1">
       <c r="A78" s="9" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="79" spans="1:29" ht="24" customHeight="1">
@@ -11591,10 +11538,10 @@
         <v>46</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="80" spans="1:29" ht="24" customHeight="1">
@@ -11602,10 +11549,10 @@
     </row>
     <row r="82" spans="1:29" ht="24" customHeight="1">
       <c r="A82" s="9" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="83" spans="1:29" ht="24" customHeight="1">
@@ -11613,10 +11560,10 @@
         <v>96</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="84" spans="1:29" ht="24" customHeight="1">
@@ -11624,10 +11571,10 @@
     </row>
     <row r="86" spans="1:29" ht="24" customHeight="1">
       <c r="A86" s="9" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="87" spans="1:29" ht="24" customHeight="1">
@@ -11635,10 +11582,10 @@
         <v>62</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="88" spans="1:29" ht="24" customHeight="1">
@@ -11649,13 +11596,13 @@
     <row r="89" spans="1:29" ht="24" customHeight="1">
       <c r="B89" s="11"/>
       <c r="AA89" s="6" t="s">
+        <v>863</v>
+      </c>
+      <c r="AB89" s="6" t="s">
+        <v>864</v>
+      </c>
+      <c r="AC89" s="6" t="s">
         <v>865</v>
-      </c>
-      <c r="AB89" s="6" t="s">
-        <v>866</v>
-      </c>
-      <c r="AC89" s="6" t="s">
-        <v>867</v>
       </c>
     </row>
   </sheetData>

</xml_diff>